<commit_message>
Update Purchase Entries Excel Template
</commit_message>
<xml_diff>
--- a/GST Tally Helper/Resources/PurchaseEntries.xlsx
+++ b/GST Tally Helper/Resources/PurchaseEntries.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Purchase Entries" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <t>Purchase</t>
   </si>
   <si>
-    <t>Journel</t>
-  </si>
-  <si>
     <t>Receipt</t>
   </si>
   <si>
     <t>Sales</t>
+  </si>
+  <si>
+    <t>Journal</t>
   </si>
 </sst>
 </file>
@@ -485,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="PurchaseEntries"/>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9549,15 +9549,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$A$2:$A$5</xm:f>
+            <xm:f>Lists!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1000</xm:sqref>
+          <xm:sqref>L2:L1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$B$2:$B$6</xm:f>
+            <xm:f>Lists!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1000</xm:sqref>
+          <xm:sqref>E2:E1000</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9567,11 +9567,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="PurchaseEntries"/>
+  <sheetPr codeName="Lists"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9589,7 +9589,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -9597,15 +9597,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -9613,19 +9613,22 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="d21fR0r3KgyL3lkHKpRZWaCivA90GiCHWm450XZ7Yk5eGF28VFivI9zgx+5vm3V7uEeQ+m60fk8VAZ0CDylkwg==" saltValue="fJn1XwHoGPUQUsCKc8+IkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>